<commit_message>
:bug: develop Fix product importing
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -892,8 +892,8 @@
   </sheetPr>
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1090,7 +1090,10 @@
       <c r="I4" s="18"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="L4" s="20" t="n">
+        <f aca="false">J4*K4</f>
+        <v>0</v>
+      </c>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
@@ -1143,7 +1146,10 @@
       <c r="I5" s="18"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="L5" s="20" t="n">
+        <f aca="false">J5*K5</f>
+        <v>0</v>
+      </c>
       <c r="M5" s="20"/>
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>

</xml_diff>

<commit_message>
:sparkles: feature/SRM-236 Remade the negotiation comparator menu from scratch
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -465,13 +465,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0_ "/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -513,7 +514,15 @@
       <b val="true"/>
       <u val="single"/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF1C1C1C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF1C1C1C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -523,6 +532,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -711,7 +725,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -752,19 +766,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,27 +794,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -879,7 +897,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF366092"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF1C1C1C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -893,7 +911,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1089,7 +1107,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="20" t="n">
         <f aca="false">J4*K4</f>
         <v>0</v>
@@ -1145,7 +1163,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="K5" s="23"/>
       <c r="L5" s="20" t="n">
         <f aca="false">J5*K5</f>
         <v>0</v>

</xml_diff>

<commit_message>
:sparkles: feature/SRM-236 Allow to upload product images with the excel file
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -325,12 +325,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="AK2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Please inster the Harmonized System Code for each product</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t xml:space="preserve">SUPPLIER</t>
   </si>
@@ -438,6 +453,9 @@
   </si>
   <si>
     <t xml:space="preserve">CÓDIGO INTERNO ASIGNADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGEN</t>
   </si>
   <si>
     <t xml:space="preserve">PCS/UNIT</t>
@@ -472,7 +490,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -532,11 +550,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -818,7 +831,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,10 +921,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK4" activeCellId="0" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1040,6 +1053,9 @@
       </c>
       <c r="AJ2" s="16" t="s">
         <v>34</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1056,25 +1072,25 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R3" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1093,6 +1109,7 @@
       <c r="AH3" s="15"/>
       <c r="AI3" s="15"/>
       <c r="AJ3" s="16"/>
+      <c r="AK3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="n">
@@ -1148,6 +1165,7 @@
       <c r="AH4" s="21"/>
       <c r="AI4" s="21"/>
       <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="n">
@@ -1204,9 +1222,10 @@
       <c r="AH5" s="21"/>
       <c r="AI5" s="21"/>
       <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="M1:O1"/>
@@ -1240,6 +1259,7 @@
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK2:AK3"/>
   </mergeCells>
   <conditionalFormatting sqref="V1:V5">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">

</xml_diff>

<commit_message>
:sparkles: feature/SRM-236 Show product image on the products table
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -11,9 +11,9 @@
     <sheet name="CREACION PRODUCTO" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_791D144D_484B_4269_9538_661214866A39_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$I:$I,'creacion producto'!#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_791D144D_484B_4269_9538_661214866A39_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$J:$J,'creacion producto'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_791D144D_484B_4269_9538_661214866A39_.wvu.Rows" vbProcedure="false">'creacion producto'!#ref!,'creacion producto'!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$M:$Z</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$N:$AA</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Rows" vbProcedure="false">'creacion producto'!#ref!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -162,11 +162,26 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">Please indicate the shelf life of the product</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">Please indicate the total number of pieces for each product</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="N3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0">
+    <comment ref="O3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0">
+    <comment ref="P3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0">
+    <comment ref="Q3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0">
+    <comment ref="R3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0">
+    <comment ref="S3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0">
+    <comment ref="U2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0">
+    <comment ref="V2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ2" authorId="0">
+    <comment ref="AK2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK2" authorId="0">
+    <comment ref="AL2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t xml:space="preserve">SUPPLIER</t>
   </si>
@@ -375,6 +390,9 @@
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGEN</t>
   </si>
   <si>
     <t xml:space="preserve">SHELF LIFE (Month*)</t>
@@ -453,9 +471,6 @@
   </si>
   <si>
     <t xml:space="preserve">CÓDIGO INTERNO ASIGNADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGEN</t>
   </si>
   <si>
     <t xml:space="preserve">PCS/UNIT</t>
@@ -738,7 +753,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -747,6 +762,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,6 +775,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -921,314 +944,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK4" activeCellId="0" sqref="AK4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="76.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="2" style="1" width="11.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="37" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="10" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="38" style="1" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="2" t="s">
+    <row r="1" s="2" customFormat="true" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="M1" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="AMJ1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="10" t="s">
+      <c r="Q2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Y2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="Z2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AD2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AF2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AG2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="15" t="s">
+      <c r="AH2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="15" t="s">
+      <c r="AI2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="16" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AK2" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="AL2" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11" t="s">
+    <row r="3" customFormat="false" ht="38.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="R3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="S3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="5"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="17"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="n">
+    <row r="4" customFormat="false" ht="76.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="20" t="n">
-        <f aca="false">J4*K4</f>
+      <c r="K4" s="22"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="22" t="n">
+        <f aca="false">K4*L4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="22" t="n">
-        <f aca="false">IFERROR(J4/O4,0)</f>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="24" t="n">
+        <f aca="false">IFERROR(K4/P4,0)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22" t="n">
-        <f aca="false">S4*V4</f>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24" t="n">
+        <f aca="false">T4*W4</f>
         <v>0</v>
       </c>
-      <c r="Y4" s="22" t="n">
-        <f aca="false">V4*T4</f>
+      <c r="Z4" s="24" t="n">
+        <f aca="false">W4*U4</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="22" t="n">
-        <f aca="false">V4*U4</f>
+      <c r="AA4" s="24" t="n">
+        <f aca="false">W4*V4</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="21"/>
-      <c r="AF4" s="21"/>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="21"/>
-      <c r="AI4" s="21"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="21"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
     </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="n">
+    <row r="5" customFormat="false" ht="76.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="n">
         <f aca="false">A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="20" t="n">
-        <f aca="false">J5*K5</f>
+      <c r="K5" s="22"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="22" t="n">
+        <f aca="false">K5*L5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="22" t="n">
-        <f aca="false">IFERROR(J5/O5,0)</f>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="24" t="n">
+        <f aca="false">IFERROR(K5/P5,0)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="22"/>
-      <c r="X5" s="22" t="n">
-        <f aca="false">S5*V5</f>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24" t="n">
+        <f aca="false">T5*W5</f>
         <v>0</v>
       </c>
-      <c r="Y5" s="22" t="n">
-        <f aca="false">V5*T5</f>
+      <c r="Z5" s="24" t="n">
+        <f aca="false">W5*U5</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="22" t="n">
-        <f aca="false">V5*U5</f>
+      <c r="AA5" s="24" t="n">
+        <f aca="false">W5*V5</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="21"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="23"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="23"/>
+      <c r="AL5" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1241,8 +1275,8 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="Q2:T2"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
@@ -1260,10 +1294,11 @@
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
     <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
   </mergeCells>
-  <conditionalFormatting sqref="V1:V5">
+  <conditionalFormatting sqref="W1:W5">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>($V1-INT($V1)&gt;0)</formula>
+      <formula>($W1-INT($W1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
:sparkles: feature/SRM-236 Export product images within the excel
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -505,7 +505,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -561,6 +561,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -753,7 +760,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -839,6 +846,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,23 +957,23 @@
   </sheetPr>
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="76.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="83.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="10" style="1" width="11.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="38" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="22.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="38.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1143,7 +1154,7 @@
       <c r="AK3" s="18"/>
       <c r="AL3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="76.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="83.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="n">
         <v>1</v>
       </c>
@@ -1154,53 +1165,53 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="22" t="n">
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="23" t="n">
         <f aca="false">K4*L4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="24" t="n">
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25" t="n">
         <f aca="false">IFERROR(K4/P4,0)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24" t="n">
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25" t="n">
         <f aca="false">T4*W4</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="24" t="n">
+      <c r="Z4" s="25" t="n">
         <f aca="false">W4*U4</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="24" t="n">
+      <c r="AA4" s="25" t="n">
         <f aca="false">W4*V4</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="23"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="76.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="83.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="n">
         <f aca="false">A4+1</f>
         <v>2</v>
@@ -1214,49 +1225,49 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="22" t="n">
+      <c r="K5" s="23"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="23" t="n">
         <f aca="false">K5*L5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="24" t="n">
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25" t="n">
         <f aca="false">IFERROR(K5/P5,0)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24" t="n">
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25" t="n">
         <f aca="false">T5*W5</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="24" t="n">
+      <c r="Z5" s="25" t="n">
         <f aca="false">W5*U5</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="24" t="n">
+      <c r="AA5" s="25" t="n">
         <f aca="false">W5*V5</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="23"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>

<commit_message>
:bug: feature/SRM-236 New format was lost
</commit_message>
<xml_diff>
--- a/public/templates/productos.xlsx
+++ b/public/templates/productos.xlsx
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_791D144D_484B_4269_9538_661214866A39_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$J:$J,'creacion producto'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_791D144D_484B_4269_9538_661214866A39_.wvu.Rows" vbProcedure="false">'creacion producto'!#ref!,'creacion producto'!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$N:$AA</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Cols" vbProcedure="false">'CREACION PRODUCTO'!$N:$AB</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_87435953_4909_431B_85F6_2691EFE020C1_.wvu.Rows" vbProcedure="false">'creacion producto'!#ref!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -147,25 +147,25 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">Please indicate the main features of each product</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">Please indicate the shelf life of the product</t>
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Please indicate the shelf life of the product</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="K2" authorId="0">
       <text>
         <r>
@@ -236,11 +236,26 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">Please indicate the quantity of pieces contained in the intermediate packaging, if applicable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">Please insert the number of pieces by carton.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0">
+    <comment ref="R3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0">
+    <comment ref="S3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0">
+    <comment ref="T3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0">
+    <comment ref="V2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0">
+    <comment ref="W2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK2" authorId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -333,25 +348,10 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="0"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Para ser llenado por OyM</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AL2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Please inster the Harmonized System Code for each product</t>
         </r>
       </text>
     </comment>
@@ -360,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t xml:space="preserve">SUPPLIER</t>
   </si>
@@ -410,7 +410,10 @@
     <t xml:space="preserve">UNIT</t>
   </si>
   <si>
-    <t xml:space="preserve">INNER</t>
+    <t xml:space="preserve">INNER 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INNER 2</t>
   </si>
   <si>
     <t xml:space="preserve">OUTER</t>
@@ -461,16 +464,34 @@
     <t xml:space="preserve">NUM REFERENCIA EMPAQUE </t>
   </si>
   <si>
+    <t xml:space="preserve">U/M UNIT</t>
+  </si>
+  <si>
     <t xml:space="preserve">CÓDIGO DE BARRAS UNIT</t>
   </si>
   <si>
-    <t xml:space="preserve">CÓDIGO DE BARRAS INNER</t>
+    <t xml:space="preserve">U/M INNER 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CÓDIGO DE BARRAS INNER 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U/M INNER 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CÓDIGO DE BARRAS INNER 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U/M OUTER</t>
   </si>
   <si>
     <t xml:space="preserve">CÓDIGO DE BARRAS OUTER</t>
   </si>
   <si>
     <t xml:space="preserve">CÓDIGO INTERNO ASIGNADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPCION ASIGNADA SISTEMA</t>
   </si>
   <si>
     <t xml:space="preserve">PCS/UNIT</t>
@@ -505,7 +526,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -567,13 +588,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -585,7 +599,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -760,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -769,10 +783,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -785,10 +795,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -846,10 +852,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -955,325 +957,362 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="83.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="88.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="10" style="1" width="11.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="38" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="10" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="45" style="1" width="11.42"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="22.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="3" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="N1" s="5" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="N1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="AMJ1" s="6"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+    <row r="2" customFormat="false" ht="43.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="12" t="s">
+      <c r="R2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="X2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="Z2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AB2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="16" t="s">
+      <c r="AC2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="16" t="s">
+      <c r="AD2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="16" t="s">
+      <c r="AE2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="16" t="s">
+      <c r="AF2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="AG2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="AH2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AI2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="AJ2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="18" t="s">
+      <c r="AK2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AL2" s="7" t="s">
-        <v>10</v>
+      <c r="AL2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR2" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="16"/>
-      <c r="AD3" s="16"/>
-      <c r="AE3" s="16"/>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="7"/>
+    <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
+      <c r="AN3" s="15"/>
+      <c r="AO3" s="15"/>
+      <c r="AP3" s="15"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
     </row>
-    <row r="4" customFormat="false" ht="83.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="n">
+    <row r="4" customFormat="false" ht="88.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="23" t="n">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20" t="n">
         <f aca="false">K4*L4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="25" t="n">
-        <f aca="false">IFERROR(K4/P4,0)</f>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="22" t="n">
+        <f aca="false">IFERROR(K4/Q4,0)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25" t="n">
-        <f aca="false">T4*W4</f>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22" t="n">
+        <f aca="false">U4*X4</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="25" t="n">
-        <f aca="false">W4*U4</f>
+      <c r="AA4" s="22" t="n">
+        <f aca="false">X4*V4</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="25" t="n">
-        <f aca="false">W4*V4</f>
+      <c r="AB4" s="22" t="n">
+        <f aca="false">X4*W4</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
     </row>
-    <row r="5" customFormat="false" ht="83.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="n">
+    <row r="5" customFormat="false" ht="88.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="n">
         <f aca="false">A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="23" t="n">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="20" t="n">
         <f aca="false">K5*L5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="25" t="n">
-        <f aca="false">IFERROR(K5/P5,0)</f>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="22" t="n">
+        <f aca="false">IFERROR(K5/Q5,0)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25" t="n">
-        <f aca="false">T5*W5</f>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22" t="n">
+        <f aca="false">U5*X5</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="25" t="n">
-        <f aca="false">W5*U5</f>
+      <c r="AA5" s="22" t="n">
+        <f aca="false">X5*V5</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="25" t="n">
-        <f aca="false">W5*V5</f>
+      <c r="AB5" s="22" t="n">
+        <f aca="false">X5*W5</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="21"/>
+      <c r="AR5" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="40">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1287,8 +1326,7 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="X2:X3"/>
@@ -1306,10 +1344,16 @@
     <mergeCell ref="AJ2:AJ3"/>
     <mergeCell ref="AK2:AK3"/>
     <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
   </mergeCells>
-  <conditionalFormatting sqref="W1:W5">
+  <conditionalFormatting sqref="X1:X5">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>($W1-INT($W1)&gt;0)</formula>
+      <formula>($X1-INT($X1)&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>